<commit_message>
Adding execution time stamp and acronym mappings
</commit_message>
<xml_diff>
--- a/odm_quote_forecast/anchored_results/NPI PTI Forecasts.xlsx
+++ b/odm_quote_forecast/anchored_results/NPI PTI Forecasts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,7 +524,7 @@
         <v>202241</v>
       </c>
       <c r="G2" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -551,12 +551,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SBDPFKBP010T</t>
+          <t>SBBPH2EX019TES1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FAIRVIEW HARBOR PRQ1</t>
+          <t>NPSG PATHFINDING</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -566,17 +566,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>FAIRVIEW</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>9.91</v>
+        <v>76.22</v>
       </c>
       <c r="F3" t="n">
         <v>202241</v>
       </c>
       <c r="G3" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -585,30 +585,30 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4900001042.0, 4900001043.0</t>
+          <t>4900001409.0</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>20221122.0</t>
+          <t>20230303.0</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>9.91</v>
+        <v>76.22</v>
       </c>
       <c r="L3" t="n">
-        <v>356.76</v>
+        <v>2439.04</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SBFPF2BU012TES1</t>
+          <t>SBDPFKBP010T</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+          <t>FAIRVIEW HARBOR PRQ1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -618,17 +618,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ1</t>
+          <t>FAIRVIEW</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>36.83777777777778</v>
+        <v>9.91</v>
       </c>
       <c r="F4" t="n">
         <v>202241</v>
       </c>
       <c r="G4" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -637,30 +637,30 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>4900001071.0, 4900000515.0, 4900001005.0, 4900001013.0, 4900001015.0, 4900001016.0, 4900001068.0, 4900001111.0, 4900001125.0</t>
+          <t>4900001042.0, 4900001043.0</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>20220831.0, 20220829.0, 20220905.0, 20221117.0, 20221201.0, 20221222.0</t>
+          <t>20221122.0</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>39.19898245614035</v>
+        <v>9.91</v>
       </c>
       <c r="L4" t="n">
-        <v>3663.974444444444</v>
+        <v>356.76</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SBFPF2BU038TES1</t>
+          <t>SBDPFKBP010TES1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+          <t>FAIRVIEW HARBOR PRQ1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -670,17 +670,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ1</t>
+          <t>FAIRVIEW</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>47.97</v>
+        <v>9.590000000000002</v>
       </c>
       <c r="F5" t="n">
         <v>202241</v>
       </c>
       <c r="G5" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -689,30 +689,30 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>4900001096.0, 4900001097.0</t>
+          <t>4900001275.0, 4900001276.0, 4900001277.0, 4900001278.0, 4900001279.0, 4900001415.0</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>20221014.0</t>
+          <t>20230206.0, 20230306.0</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>47.97000000000001</v>
+        <v>9.573</v>
       </c>
       <c r="L5" t="n">
-        <v>3837.6</v>
+        <v>510.56</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SBFPF2BU076TES1</t>
+          <t>SBDPFKBP020TES1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+          <t>FAIRVIEW HARBOR PRQ1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -722,17 +722,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ1</t>
+          <t>FAIRVIEW</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>49.235</v>
+        <v>9.57</v>
       </c>
       <c r="F6" t="n">
         <v>202241</v>
       </c>
       <c r="G6" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -741,30 +741,30 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>4900001093.0, 4900001094.0</t>
+          <t>4900001284.0, 4900001285.0, 4900001282.0, 4900001283.0</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>20221014.0</t>
+          <t>20230206.0</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>49.23499999999999</v>
+        <v>9.57</v>
       </c>
       <c r="L6" t="n">
-        <v>3347.98</v>
+        <v>229.68</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SBFPF2BU153TES1</t>
+          <t>SBDPFKBP512GES1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+          <t>FAIRVIEW HARBOR PRQ1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -774,17 +774,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ1</t>
+          <t>FAIRVIEW</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>55.19</v>
+        <v>9.570000000000002</v>
       </c>
       <c r="F7" t="n">
         <v>202241</v>
       </c>
       <c r="G7" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -793,30 +793,30 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>4900001091.0, 4900001092.0</t>
+          <t>4900001269.0, 4900001270.0, 4900001271.0, 4900001272.0, 4900001273.0, 4900001274.0, 4900001326.0</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>20221014.0</t>
+          <t>20230206.0, 20230213.0</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>55.02</v>
+        <v>9.57</v>
       </c>
       <c r="L7" t="n">
-        <v>1980.72</v>
+        <v>1093.714285714286</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SBFPF2BU307TES1</t>
+          <t>SBFPF2BU012TES1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR EE PRQ2</t>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -826,17 +826,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ2</t>
+          <t>ADPRRR EE PRQ1</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>106.09</v>
+        <v>37.03642857142857</v>
       </c>
       <c r="F8" t="n">
         <v>202241</v>
       </c>
       <c r="G8" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -845,30 +845,30 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>4900000524.0, 4900000525.0, 4900000526.0, 4900000527.0</t>
+          <t>4900001071.0, 4900000515.0, 4900001005.0, 4900001013.0, 4900001015.0, 4900001016.0, 4900001068.0, 4900001111.0, 4900001125.0, 4900001130.0, 4900001131.0, 4900001004.0, 4900001203.0, 4900001219.0</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>20220912.0</t>
+          <t>20220831.0, 20220829.0, 20220905.0, 20221117.0, 20221201.0, 20221222.0, 20221124.0, 20230112.0</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>106.0923188405797</v>
+        <v>37.78814415907208</v>
       </c>
       <c r="L8" t="n">
-        <v>5490.2775</v>
+        <v>3219.352142857143</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SBFPF2BV025TES1</t>
+          <t>SBFPF2BU038TES1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ1</t>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -878,17 +878,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ADPRRR VE</t>
+          <t>ADPRRR EE PRQ1</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>48.47</v>
+        <v>46.20625</v>
       </c>
       <c r="F9" t="n">
         <v>202241</v>
       </c>
       <c r="G9" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -897,30 +897,30 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>4900000523.0, 4900001069.0, 4900001070.0</t>
+          <t>4900001096.0, 4900001097.0, 4900001136.0, 4900001137.0, 4900001294.0, 4900001295.0, 4900001370.0, 4900001371.0</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>20220905.0, 20221201.0</t>
+          <t>20221014.0, 20221124.0, 20230118.0, 20230216.0</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>48.38795580110497</v>
+        <v>45.38122529644269</v>
       </c>
       <c r="L9" t="n">
-        <v>11677.62666666667</v>
+        <v>5740.725</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SBFPF2BV025TES1</t>
+          <t>SBFPF2BU038TESF</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ4</t>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -930,17 +930,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ4</t>
+          <t>ADPRRR EE PRQ1</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>49.12</v>
+        <v>44.12</v>
       </c>
       <c r="F10" t="n">
         <v>202241</v>
       </c>
       <c r="G10" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -949,30 +949,30 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>4900001028.0</t>
+          <t>4900001372.0, 4900001373.0</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>20220916.0</t>
+          <t>20230216.0</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>49.12</v>
+        <v>44.13888888888889</v>
       </c>
       <c r="L10" t="n">
-        <v>7073.280000000001</v>
+        <v>794.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SBFPF2BV025TES1</t>
+          <t>SBFPF2BU076TES1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>NPSG PATHFINDING</t>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -982,17 +982,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>ADPRRR EE PRQ1</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>110.21</v>
+        <v>46.97</v>
       </c>
       <c r="F11" t="n">
         <v>202241</v>
       </c>
       <c r="G11" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1001,30 +1001,30 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>4900001047.0, 4900001049.0</t>
+          <t>4900001093.0, 4900001094.0, 4900001134.0, 4900001135.0, 4900001292.0, 4900001293.0, 4900001366.0, 4900001367.0</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>20221116.0</t>
+          <t>20221014.0, 20221124.0, 20230118.0, 20230216.0</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>81.92428571428572</v>
+        <v>45.23199178644763</v>
       </c>
       <c r="L11" t="n">
-        <v>1146.94</v>
+        <v>11013.99</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SBFPF2BV076TES1</t>
+          <t>SBFPF2BU076TESF</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1034,17 +1034,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>ADPRRR EE PRQ1</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>48.67999999999999</v>
+        <v>44.385</v>
       </c>
       <c r="F12" t="n">
         <v>202241</v>
       </c>
       <c r="G12" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1053,30 +1053,30 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>4900001017.0, 4900001018.0</t>
+          <t>4900001368.0, 4900001369.0</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>20221101.0</t>
+          <t>20230216.0</t>
         </is>
       </c>
       <c r="K12" t="n">
-        <v>48.67999999999999</v>
+        <v>44.38499999999999</v>
       </c>
       <c r="L12" t="n">
-        <v>4283.839999999999</v>
+        <v>1065.24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SBFPF2BV153TES1</t>
+          <t>SBFPF2BU153TES1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1086,17 +1086,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>ADPRRR EE PRQ1</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>55.70000000000001</v>
+        <v>47.16166666666667</v>
       </c>
       <c r="F13" t="n">
         <v>202241</v>
       </c>
       <c r="G13" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1105,30 +1105,30 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>4900001021.0, 4900001022.0, 4900001023.0</t>
+          <t>4900001091.0, 4900001092.0, 4900001140.0, 4900001141.0, 4900001296.0, 4900001297.0, 4900001410.0, 4900001363.0, 4900001364.0, 4900001414.0, 4900001453.0, 4900001455.0</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>20221101.0</t>
+          <t>20221014.0, 20221201.0, 20230118.0, 20230309.0, 20230216.0, 20230313.0, 20230316.0</t>
         </is>
       </c>
       <c r="K13" t="n">
-        <v>55.7</v>
+        <v>44.69365595611286</v>
       </c>
       <c r="L13" t="n">
-        <v>3639.066666666667</v>
+        <v>19009.70166666667</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>SBFPF2BV153TES1</t>
+          <t>SBFPF2BU153TESF</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ4</t>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1138,17 +1138,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ4</t>
+          <t>ADPRRR EE PRQ1</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>54.65</v>
+        <v>45.065</v>
       </c>
       <c r="F14" t="n">
         <v>202241</v>
       </c>
       <c r="G14" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1157,30 +1157,30 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>4900001030.0</t>
+          <t>4900001362.0, 4900001365.0</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>20220915.0</t>
+          <t>20230216.0</t>
         </is>
       </c>
       <c r="K14" t="n">
-        <v>54.65</v>
+        <v>45.0743</v>
       </c>
       <c r="L14" t="n">
-        <v>3934.8</v>
+        <v>4507.43</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>SBFPF2BV307TES1</t>
+          <t>SBFPF2BU307TES1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+          <t>ARBORDALE PLUS RRR EE PRQ2</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1190,17 +1190,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>138.75</v>
+        <v>107.35</v>
       </c>
       <c r="F15" t="n">
         <v>202241</v>
       </c>
       <c r="G15" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1209,30 +1209,30 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>4900001019.0, 4900001020.0</t>
+          <t>4900000524.0, 4900000525.0, 4900000526.0, 4900000527.0, 4900001144.0, 4900001145.0, 4900001146.0, 4900001147.0, 4900001317.0, 4900001318.0, 4900001417.0, 4900001418.0</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>20221101.0, 20221107.0</t>
+          <t>20220912.0, 20221124.0, 20230213.0, 20230223.0</t>
         </is>
       </c>
       <c r="K15" t="n">
-        <v>138.75</v>
+        <v>109.6345625</v>
       </c>
       <c r="L15" t="n">
-        <v>5550</v>
+        <v>4385.382500000001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SBFPF2BV614TES1</t>
+          <t>SBFPF2BV025TES1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+          <t>ARBORDALE PLUS RRR VE PRQ1</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1242,17 +1242,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>ADPRRR VE</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>115.555</v>
+        <v>47.14166666666667</v>
       </c>
       <c r="F16" t="n">
         <v>202241</v>
       </c>
       <c r="G16" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1261,30 +1261,30 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>4900000908.0, 4900000909.0, 4900000910.0, 4900000911.0</t>
+          <t>4900000523.0, 4900001069.0, 4900001070.0, 4900001198.0, 4900001304.0, 4900001290.0</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>20221004.0, 20220927.0, 20221031.0</t>
+          <t>20220905.0, 20221201.0, 20230106.0, 20230208.0</t>
         </is>
       </c>
       <c r="K16" t="n">
-        <v>116.8689312977099</v>
+        <v>48.06676616915423</v>
       </c>
       <c r="L16" t="n">
-        <v>3827.4575</v>
+        <v>6440.946666666667</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SBFPFABU038TES1</t>
+          <t>SBFPF2BV025TES1</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+          <t>ARBORDALE PLUS RRR VE PRQ4</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1294,17 +1294,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ1</t>
+          <t>ADPRRR VE PRQ4</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>59.91666666666666</v>
+        <v>49.12</v>
       </c>
       <c r="F17" t="n">
         <v>202241</v>
       </c>
       <c r="G17" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1313,30 +1313,30 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>4900001014.0, 4900001089.0, 4900001090.0</t>
+          <t>4900001028.0</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>20221117.0, 20221014.0</t>
+          <t>20220916.0</t>
         </is>
       </c>
       <c r="K17" t="n">
-        <v>59.79833333333334</v>
+        <v>49.12</v>
       </c>
       <c r="L17" t="n">
-        <v>956.7733333333334</v>
+        <v>7073.280000000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SBFPFABU076TES1</t>
+          <t>SBFPF2BV025TES1</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+          <t>NPSG PATHFINDING</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1346,17 +1346,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ1</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>59.40000000000001</v>
+        <v>110.21</v>
       </c>
       <c r="F18" t="n">
         <v>202241</v>
       </c>
       <c r="G18" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1365,30 +1365,30 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>4900001095.0</t>
+          <t>4900001047.0, 4900001049.0</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>20221014.0</t>
+          <t>20221116.0</t>
         </is>
       </c>
       <c r="K18" t="n">
-        <v>59.4</v>
+        <v>81.92428571428572</v>
       </c>
       <c r="L18" t="n">
-        <v>1188</v>
+        <v>1146.94</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SBFPFABU153TES1</t>
+          <t>SBFPF2BV076TES1</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1398,17 +1398,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ1</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>61.29</v>
+        <v>46.752</v>
       </c>
       <c r="F19" t="n">
         <v>202241</v>
       </c>
       <c r="G19" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1417,30 +1417,30 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>4900001088.0, 4900001112.0</t>
+          <t>4900001017.0, 4900001018.0, 4900001183.0, 4900001386.0, 4900001387.0</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>20221014.0, 20221207.0</t>
+          <t>20221101.0, 20221228.0, 20230118.0</t>
         </is>
       </c>
       <c r="K19" t="n">
-        <v>61.29</v>
+        <v>45.94557692307691</v>
       </c>
       <c r="L19" t="n">
-        <v>3099</v>
+        <v>3822.672</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SBFPFABU307TES1</t>
+          <t>SBFPF2BV153TES1</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR EE PRQ2</t>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1450,17 +1450,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ2</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>104.495</v>
+        <v>52.13666666666666</v>
       </c>
       <c r="F20" t="n">
         <v>202241</v>
       </c>
       <c r="G20" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1469,30 +1469,30 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>4900000530.0, 4900000531.0, 4900000532.0, 4900000533.0</t>
+          <t>4900001021.0, 4900001022.0, 4900001023.0, 4900001182.0, 4900001382.0, 4900001383.0</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>20220912.0</t>
+          <t>20221101.0, 20221228.0, 20230118.0</t>
         </is>
       </c>
       <c r="K20" t="n">
-        <v>104.495</v>
+        <v>51.42674418604651</v>
       </c>
       <c r="L20" t="n">
-        <v>4806.77</v>
+        <v>2948.466666666667</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SBFPFABV076TES1</t>
+          <t>SBFPF2BV153TES1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+          <t>ARBORDALE PLUS RRR VE PRQ4</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1502,17 +1502,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>ADPRRR VE PRQ4</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>60.595</v>
+        <v>54.65</v>
       </c>
       <c r="F21" t="n">
         <v>202241</v>
       </c>
       <c r="G21" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1521,30 +1521,30 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>NaN, 4900001210.0</t>
+          <t>4900001030.0</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>20220823.0, 20221228.0</t>
+          <t>20220915.0</t>
         </is>
       </c>
       <c r="K21" t="n">
-        <v>60.595</v>
+        <v>54.65</v>
       </c>
       <c r="L21" t="n">
-        <v>1454.28</v>
+        <v>3934.8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SBFPFABV153TES1</t>
+          <t>SBFPF2BV153TES1</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+          <t>NPSG PATHFINDING</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1554,17 +1554,17 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>60.64</v>
+        <v>78.21000000000001</v>
       </c>
       <c r="F22" t="n">
         <v>202241</v>
       </c>
       <c r="G22" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -1573,30 +1573,30 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>4900001048.0</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>20220823.0</t>
+          <t>20221116.0</t>
         </is>
       </c>
       <c r="K22" t="n">
-        <v>60.522</v>
+        <v>78.21000000000001</v>
       </c>
       <c r="L22" t="n">
-        <v>1815.66</v>
+        <v>312.84</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SBFPFABV153TES1</t>
+          <t>SBFPF2BV307TES1</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ4</t>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1606,17 +1606,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ4</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>60.13</v>
+        <v>114.19</v>
       </c>
       <c r="F23" t="n">
         <v>202241</v>
       </c>
       <c r="G23" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1625,25 +1625,25 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>4900001029.0</t>
+          <t>4900001019.0, 4900001020.0, 4900001205.0, 4900001384.0, 4900001385.0</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>20220915.0</t>
+          <t>20221101.0, 20221107.0, 20230106.0, 20230131.0</t>
         </is>
       </c>
       <c r="K23" t="n">
-        <v>60.13</v>
+        <v>109.2489547038327</v>
       </c>
       <c r="L23" t="n">
-        <v>1683.64</v>
+        <v>6270.889999999999</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>SBFPFABV307TES1</t>
+          <t>SBFPF2BV614TES1</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1662,13 +1662,13 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>105.52</v>
+        <v>116.8471428571429</v>
       </c>
       <c r="F24" t="n">
         <v>202241</v>
       </c>
       <c r="G24" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1677,30 +1677,30 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>4900001101.0, 4900001102.0</t>
+          <t>4900000908.0, 4900000909.0, 4900000910.0, 4900000911.0, 4900001401.0, 4900001402.0, 4900001403.0</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>20221004.0, 20220908.0</t>
+          <t>20221004.0, 20220927.0, 20221031.0, 20230217.0</t>
         </is>
       </c>
       <c r="K24" t="n">
-        <v>105.52</v>
+        <v>111.7962893081761</v>
       </c>
       <c r="L24" t="n">
-        <v>2532.48</v>
+        <v>5078.745714285716</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SBFPFUBU038TES1</t>
+          <t>SBFPFABU038TEHP</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR EE PRQ2</t>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1710,17 +1710,17 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ2</t>
+          <t>ADPRRR EE PRQ1</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>66</v>
+        <v>52.45</v>
       </c>
       <c r="F25" t="n">
         <v>202241</v>
       </c>
       <c r="G25" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -1729,30 +1729,30 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>4900000528.0, 4900000529.0, 4900000807.0, 4900000808.0</t>
+          <t>4900001381.0</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>20220916.0, 20220912.0</t>
+          <t>20230302.0</t>
         </is>
       </c>
       <c r="K25" t="n">
-        <v>66</v>
+        <v>52.45</v>
       </c>
       <c r="L25" t="n">
-        <v>1848</v>
+        <v>5664.6</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SBFPFUBU076TES1</t>
+          <t>SBFPFABU038TES1</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR EE PRQ2</t>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1762,17 +1762,17 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ2</t>
+          <t>ADPRRR EE PRQ1</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>65.17</v>
+        <v>63.02111111111112</v>
       </c>
       <c r="F26" t="n">
         <v>202241</v>
       </c>
       <c r="G26" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -1781,30 +1781,30 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>4900000803.0, 4900000804.0, 4900000805.0, 4900000806.0</t>
+          <t>4900001014.0, 4900001089.0, 4900001090.0, 4900001132.0, 4900001133.0, 4900001300.0, 4900001301.0, 4900001377.0, 4900001378.0</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>20220912.0, 20220916.0</t>
+          <t>20221117.0, 20221014.0, 20221124.0, 20230118.0, 20230216.0</t>
         </is>
       </c>
       <c r="K26" t="n">
-        <v>65.16941176470588</v>
+        <v>64.59958333333334</v>
       </c>
       <c r="L26" t="n">
-        <v>2215.76</v>
+        <v>3445.311111111112</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SBFPFUBU153TES1</t>
+          <t>SBFPFABU076TEHP</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR EE PRQ2</t>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1814,17 +1814,17 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ2</t>
+          <t>ADPRRR EE PRQ1</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>65.86500000000001</v>
+        <v>48.48</v>
       </c>
       <c r="F27" t="n">
         <v>202241</v>
       </c>
       <c r="G27" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1833,30 +1833,30 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>4900000799.0, 4900000800.0, 4900000801.0, 4900000802.0</t>
+          <t>4900001380.0</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>20220912.0, 20220916.0</t>
+          <t>20230302.0</t>
         </is>
       </c>
       <c r="K27" t="n">
-        <v>65.86499999999999</v>
+        <v>48.48</v>
       </c>
       <c r="L27" t="n">
-        <v>1844.22</v>
+        <v>5041.92</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SBFPFWBV153TES1</t>
+          <t>SBFPFABU076TES1</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ1</t>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1866,17 +1866,17 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>ADPRRR VE</t>
+          <t>ADPRRR EE PRQ1</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>97.68666666666667</v>
+        <v>62.00285714285714</v>
       </c>
       <c r="F28" t="n">
         <v>202241</v>
       </c>
       <c r="G28" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -1885,30 +1885,30 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>4900000521.0, 4900000522.0, 4900001099.0</t>
+          <t>4900001095.0, 4900001138.0, 4900001139.0, 4900001298.0, 4900001299.0, 4900001361.0, 4900001376.0</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>20220905.0, 20221213.0</t>
+          <t>20221014.0, 20221207.0, 20221201.0, 20230118.0, 20230216.0</t>
         </is>
       </c>
       <c r="K28" t="n">
-        <v>97.53733333333334</v>
+        <v>62.60437908496733</v>
       </c>
       <c r="L28" t="n">
-        <v>11704.48</v>
+        <v>5473.411428571429</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SBFPFWBV153TES1</t>
+          <t>SBFPFABU153TEHP</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1918,17 +1918,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>ADPRRR EE PRQ1</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>98.06</v>
+        <v>49</v>
       </c>
       <c r="F29" t="n">
         <v>202241</v>
       </c>
       <c r="G29" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -1937,30 +1937,30 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>4900001026.0, 4900001027.0</t>
+          <t>4900001379.0</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>20221101.0</t>
+          <t>20230302.0</t>
         </is>
       </c>
       <c r="K29" t="n">
-        <v>98.05999999999999</v>
+        <v>49</v>
       </c>
       <c r="L29" t="n">
-        <v>2745.68</v>
+        <v>5292</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SBFPFWBV307TES1</t>
+          <t>SBFPFABU153TES1</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ1</t>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1970,17 +1970,17 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>ADPRRR VE</t>
+          <t>ADPRRR EE PRQ1</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>124.1433333333333</v>
+        <v>60.51272727272727</v>
       </c>
       <c r="F30" t="n">
         <v>202241</v>
       </c>
       <c r="G30" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -1989,30 +1989,30 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>4900001056.0, 4900000520.0, 4900001098.0</t>
+          <t>4900001088.0, 4900001112.0, 4900001142.0, 4900001143.0, 4900001187.0, 4900001195.0, 4900001324.0, 4900001325.0, 4900001374.0, 4900001375.0, 4900001413.0</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>20220905.0, 20221101.0</t>
+          <t>20221014.0, 20221207.0, 20221201.0, 20230106.0, 20230111.0, 20230118.0, 20230112.0, 20230216.0, 20230306.0</t>
         </is>
       </c>
       <c r="K30" t="n">
-        <v>134.7667415730337</v>
+        <v>61.92841145833333</v>
       </c>
       <c r="L30" t="n">
-        <v>15992.32</v>
+        <v>4664.310909090909</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SBFPFWBV307TES1</t>
+          <t>SBFPFABU307TES1</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+          <t>ARBORDALE PLUS RRR EE PRQ2</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2022,17 +2022,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>97.50999999999999</v>
+        <v>93.634</v>
       </c>
       <c r="F31" t="n">
         <v>202241</v>
       </c>
       <c r="G31" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -2041,25 +2041,25 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>4900001024.0, 4900001025.0</t>
+          <t>4900000530.0, 4900000531.0, 4900000532.0, 4900000533.0, 4900001213.0, 4900001214.0, 4900001215.0, 4900001216.0, 4900001281.0, 4900001319.0</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>20221101.0</t>
+          <t>20220912.0, 20221201.0, 20230206.0, 20230213.0</t>
         </is>
       </c>
       <c r="K31" t="n">
-        <v>97.50999999999999</v>
+        <v>94.38868686868686</v>
       </c>
       <c r="L31" t="n">
-        <v>2340.24</v>
+        <v>3737.792</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SBFPFWBV614TES1</t>
+          <t>SBFPFABV076TES1</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2078,13 +2078,13 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>99.88</v>
+        <v>58.83666666666667</v>
       </c>
       <c r="F32" t="n">
         <v>202241</v>
       </c>
       <c r="G32" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -2093,30 +2093,30 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>4900000449.0, 4900000450.0, 4900000451.0</t>
+          <t>NaN, 4900001210.0, 4900001199.0</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>20220908.0, 20220927.0</t>
+          <t>20220823.0, 20221228.0, 20230106.0</t>
         </is>
       </c>
       <c r="K32" t="n">
-        <v>99.88</v>
+        <v>60.18923076923078</v>
       </c>
       <c r="L32" t="n">
-        <v>4661.066666666667</v>
+        <v>1043.28</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SSDPF2KX012T1ES</t>
+          <t>SBFPFABV153TES1</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RR SE PRQ1</t>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2126,17 +2126,17 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>ADPRR SE PRQ1</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>28.12</v>
+        <v>61.22</v>
       </c>
       <c r="F33" t="n">
         <v>202241</v>
       </c>
       <c r="G33" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
@@ -2145,30 +2145,30 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>4900000444.0, 4900000516.0, 4900001003.0, 4900001037.0</t>
+          <t>NaN, 4900001181.0</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>20220823, 20220905, 20220912</t>
+          <t>20220823.0, 20221228.0</t>
         </is>
       </c>
       <c r="K33" t="n">
-        <v>28.09173913043478</v>
+        <v>60.638125</v>
       </c>
       <c r="L33" t="n">
-        <v>1938.33</v>
+        <v>1293.613333333333</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>SSDPF2KX012TZES</t>
+          <t>SBFPFABV153TES1</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS R SE PRQ1</t>
+          <t>ARBORDALE PLUS RRR VE PRQ4</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2178,17 +2178,17 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>ADPR SE</t>
+          <t>ADPRRR VE PRQ4</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>36.75600000000001</v>
+        <v>60.13</v>
       </c>
       <c r="F34" t="n">
         <v>202241</v>
       </c>
       <c r="G34" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
@@ -2197,30 +2197,30 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>4900000339.0, 4900001002.0, 4900001064.0, 4900001065.0, 4900001036.0</t>
+          <t>4900001029.0</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>20220808.0, 20221107.0, 20221117.0, 20221123.0, 20220905.0</t>
+          <t>20220915.0</t>
         </is>
       </c>
       <c r="K34" t="n">
-        <v>41.20394230769232</v>
+        <v>60.13</v>
       </c>
       <c r="L34" t="n">
-        <v>3428.168000000001</v>
+        <v>1683.64</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>SSDPF2KX019T1M1</t>
+          <t>SBFPFABV307TES1</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RR SE</t>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2230,17 +2230,17 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>ADPRR SE</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>42.08</v>
+        <v>105.52</v>
       </c>
       <c r="F35" t="n">
         <v>202241</v>
       </c>
       <c r="G35" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -2249,30 +2249,30 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>4900001081.0, 4900001082.0</t>
+          <t>4900001101.0, 4900001102.0</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>20221123</t>
+          <t>20221004.0, 20220908.0</t>
         </is>
       </c>
       <c r="K35" t="n">
-        <v>42.08</v>
+        <v>105.52</v>
       </c>
       <c r="L35" t="n">
-        <v>8416</v>
+        <v>2532.48</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>SSDPF2KX076T1ES</t>
+          <t>SBFPFUBU038TES1</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RR SE PRQ1</t>
+          <t>ARBORDALE PLUS RRR EE PRQ2</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2282,17 +2282,17 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>ADPRR SE PRQ1</t>
+          <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>45.31</v>
+        <v>65.06999999999999</v>
       </c>
       <c r="F36" t="n">
         <v>202241</v>
       </c>
       <c r="G36" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
@@ -2301,30 +2301,30 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>4900000798.0</t>
+          <t>4900000528.0, 4900000529.0, 4900000807.0, 4900000808.0, 4900001148.0, 4900001149.0, 4900001152.0, 4900001153.0, 4900001316.0</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>20221020</t>
+          <t>20220916.0, 20220912.0, 20221201.0, 20230213.0</t>
         </is>
       </c>
       <c r="K36" t="n">
-        <v>45.31</v>
+        <v>65.33937499999999</v>
       </c>
       <c r="L36" t="n">
-        <v>181.24</v>
+        <v>1858.542222222222</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>SSDPF2KX153T1N1</t>
+          <t>SBFPFUBU076TES1</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RR SE</t>
+          <t>ARBORDALE PLUS RRR EE PRQ2</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2334,17 +2334,17 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>ADPRR SE</t>
+          <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>104.48</v>
+        <v>63.95333333333333</v>
       </c>
       <c r="F37" t="n">
         <v>202241</v>
       </c>
       <c r="G37" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
@@ -2353,30 +2353,30 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>4900001086.0, 4900001087.0</t>
+          <t>4900000803.0, 4900000804.0, 4900000805.0, 4900000806.0, 4900001150.0, 4900001151.0, 4900001154.0, 4900001155.0, 4900001314.0</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>20221123</t>
+          <t>20220912.0, 20220916.0, 20221201.0, 20230213.0</t>
         </is>
       </c>
       <c r="K37" t="n">
-        <v>104.48</v>
+        <v>64.45371428571428</v>
       </c>
       <c r="L37" t="n">
-        <v>20896</v>
+        <v>2005.226666666667</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>SSDPFCKE064T1S1</t>
+          <t>SBFPFUBU153TES1</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RR ME</t>
+          <t>ARBORDALE PLUS RRR EE PRQ2</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2386,17 +2386,17 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ADPRR ME PRQ1</t>
+          <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>69.96499999999999</v>
+        <v>64.93900000000001</v>
       </c>
       <c r="F38" t="n">
         <v>202241</v>
       </c>
       <c r="G38" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
@@ -2405,30 +2405,30 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>4900001066.0, 4900001067.0</t>
+          <t>4900000799.0, 4900000800.0, 4900000801.0, 4900000802.0, 4900001220.0, 4900001221.0, 4900001222.0, 4900001223.0, 4900001100.0, 4900001315.0</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>20221123.0</t>
+          <t>20220912.0, 20220916.0, 20221124.0, 20221201.0, 20230213.0</t>
         </is>
       </c>
       <c r="K38" t="n">
-        <v>69.96499999999999</v>
+        <v>65.44534883720931</v>
       </c>
       <c r="L38" t="n">
-        <v>13993</v>
+        <v>2251.32</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>SSDPFUKX019T1AP</t>
+          <t>SBFPFWBV153TES1</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RR SE</t>
+          <t>ARBORDALE PLUS RRR VE PRQ1</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2438,17 +2438,17 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>ADPRR SE</t>
+          <t>ADPRRR VE</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>53.06999999999999</v>
+        <v>94.74416666666667</v>
       </c>
       <c r="F39" t="n">
         <v>202241</v>
       </c>
       <c r="G39" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -2457,30 +2457,30 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>4900001083.0</t>
+          <t>4900000521.0, 4900000522.0, 4900001099.0, 4900001197.0, 4900001240.0, 4900001204.0, 4900001242.0, 4900001302.0, 4900001320.0, 4900001462.0, 4900001524.0, 4900001496.0</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>20221123</t>
+          <t>20220905.0, 20221213.0, 20230106.0, 20230131.0, 20230112.0, 20221124.0, 20230216.0, 20230407.0, 20230324.0</t>
         </is>
       </c>
       <c r="K39" t="n">
-        <v>53.06999999999999</v>
+        <v>94.55739130434783</v>
       </c>
       <c r="L39" t="n">
-        <v>424.5599999999999</v>
+        <v>7249.400000000001</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>SSDPFUKX076T1AP</t>
+          <t>SBFPFWBV153TES1</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RR SE</t>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2490,17 +2490,17 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>ADPRR SE</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>58.67</v>
+        <v>98.06</v>
       </c>
       <c r="F40" t="n">
         <v>202241</v>
       </c>
       <c r="G40" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
@@ -2509,30 +2509,30 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>4900001084.0</t>
+          <t>4900001026.0, 4900001027.0</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>20221123</t>
+          <t>20221101.0</t>
         </is>
       </c>
       <c r="K40" t="n">
-        <v>58.67</v>
+        <v>98.05999999999999</v>
       </c>
       <c r="L40" t="n">
-        <v>469.36</v>
+        <v>2745.68</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>SSDPFWKX153T1M2</t>
+          <t>SBFPFWBV153TESF</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ARBORDALE PLUS RR SE</t>
+          <t>ARBORDALE PLUS RRR VE PRQ1</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2542,17 +2542,17 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ADPRR SE</t>
+          <t>ADPRRR VE</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>108.97</v>
+        <v>87.38000000000001</v>
       </c>
       <c r="F41" t="n">
         <v>202241</v>
       </c>
       <c r="G41" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
@@ -2561,30 +2561,30 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>4900001085.0</t>
+          <t>4900001291.0</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>20221123</t>
+          <t>20230208.0</t>
         </is>
       </c>
       <c r="K41" t="n">
-        <v>108.97</v>
+        <v>87.38000000000001</v>
       </c>
       <c r="L41" t="n">
-        <v>871.76</v>
+        <v>6990.400000000001</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>SSDPFWKX153T8M2</t>
+          <t>SBFPFWBV307TES1</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>CDR SE EDSFF</t>
+          <t>ARBORDALE PLUS RRR VE PRQ1</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2594,17 +2594,17 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>CDR SE EDSFF</t>
+          <t>ADPRRR VE</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>104.53</v>
+        <v>101.6823076923077</v>
       </c>
       <c r="F42" t="n">
         <v>202241</v>
       </c>
       <c r="G42" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -2613,30 +2613,30 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>4900000912.0</t>
+          <t>4900001056.0, 4900000520.0, 4900001098.0, 4900001196.0, 4900001208.0, 4900001241.0, 4900001303.0, 4900001305.0, 4900001321.0, 4900001456.0, 4900001461.0, 4900001495.0, 4900001498.0</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>20221028</t>
+          <t>20220905.0, 20221101.0, 20230106.0, 20230118.0, 20230131.0, 20221124.0, 20230213.0, 20230316.0, 20230216.0, 20230324.0</t>
         </is>
       </c>
       <c r="K42" t="n">
-        <v>104.53</v>
+        <v>111.4890365448505</v>
       </c>
       <c r="L42" t="n">
-        <v>1254.36</v>
+        <v>10325.6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>SSDPFWNV153TZES</t>
+          <t>SBFPFWBV307TES1</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>NPSG PATHFINDING</t>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2646,15 +2646,17 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>PF</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr"/>
+          <t>ADPRRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>97.50999999999999</v>
+      </c>
       <c r="F43" t="n">
         <v>202241</v>
       </c>
       <c r="G43" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -2663,26 +2665,30 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>9000000069.0</t>
+          <t>4900001024.0, 4900001025.0</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>20230123.0</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
+          <t>20221101.0</t>
+        </is>
+      </c>
+      <c r="K43" t="n">
+        <v>97.50999999999999</v>
+      </c>
+      <c r="L43" t="n">
+        <v>2340.24</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>SSDSC2KB038TZ01</t>
+          <t>SBFPFWBV307TES1</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>YOUNGSVILLE RR SE</t>
+          <t>ARBORDALE PLUS RRR VE PRQ4</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2692,17 +2698,17 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>YV RR SE</t>
+          <t>ADPRRR VE PRQ4</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>21.69</v>
+        <v>98.06999999999999</v>
       </c>
       <c r="F44" t="n">
         <v>202241</v>
       </c>
       <c r="G44" t="n">
-        <v>202253</v>
+        <v>202313</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -2711,71 +2717,1319 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>4900000534, 4900000535</t>
+          <t>4900001506.0</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>20220908</t>
+          <t>20230324.0</t>
         </is>
       </c>
       <c r="K44" t="n">
-        <v>21.68999999999999</v>
+        <v>98.06999999999999</v>
       </c>
       <c r="L44" t="n">
-        <v>2342.52</v>
+        <v>8630.16</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>SBFPFWBV307TESF</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS RRR VE PRQ1</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>ADPRRR VE</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>128.11</v>
+      </c>
+      <c r="F45" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G45" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>4900001322.0</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>20230213.0</t>
+        </is>
+      </c>
+      <c r="K45" t="n">
+        <v>128.11</v>
+      </c>
+      <c r="L45" t="n">
+        <v>10248.8</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>SBFPFWBV614TES1</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>ADPRRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>102.655</v>
+      </c>
+      <c r="F46" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G46" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>4900000449.0, 4900000450.0, 4900000451.0, 4900001398.0, 4900001399.0, 4900001459.0</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>20220908.0, 20220927.0, 20230324.0, 20230406.0</t>
+        </is>
+      </c>
+      <c r="K46" t="n">
+        <v>103.17046875</v>
+      </c>
+      <c r="L46" t="n">
+        <v>4401.94</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>SSDPF2KX012T1ES</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS RR SE PRQ1</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>ADPRR SE PRQ1</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>27.59857142857143</v>
+      </c>
+      <c r="F47" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G47" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>4900000444.0, 4900000516.0, 4900001003.0, 4900001037.0, 4900001129.0, 4900001358.0, 4900001359.0</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>20220823, 20220905, 20220912, 20221124, 20230214</t>
+        </is>
+      </c>
+      <c r="K47" t="n">
+        <v>27.70725490196078</v>
+      </c>
+      <c r="L47" t="n">
+        <v>1614.937142857143</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>SSDPF2KX012TZES</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS R SE PRQ1</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>ADPR SE</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>36.835</v>
+      </c>
+      <c r="F48" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G48" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>4900000339.0, 4900001002.0, 4900001064.0, 4900001065.0, 4900001036.0, 4900001175.0, 4900001176.0, 4900001217.0</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>20220808.0, 20221107.0, 20221117.0, 20221123.0, 20220905.0, 20221213.0, 20230111.0</t>
+        </is>
+      </c>
+      <c r="K48" t="n">
+        <v>41.21995145631069</v>
+      </c>
+      <c r="L48" t="n">
+        <v>4245.655000000001</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>SSDPF2KX019T1M1</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS RR SE</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>ADPRR SE</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>42.08</v>
+      </c>
+      <c r="F49" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G49" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>4900001081.0, 4900001082.0</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>20221123</t>
+        </is>
+      </c>
+      <c r="K49" t="n">
+        <v>42.08</v>
+      </c>
+      <c r="L49" t="n">
+        <v>8416</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>SSDPF2KX076T1ES</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS RR SE PRQ1</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>ADPRR SE PRQ1</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>45.31</v>
+      </c>
+      <c r="F50" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G50" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>4900000798.0</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>20221020</t>
+        </is>
+      </c>
+      <c r="K50" t="n">
+        <v>45.31</v>
+      </c>
+      <c r="L50" t="n">
+        <v>181.24</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>SSDPF2KX153T1N1</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS RR SE</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>ADPRR SE</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>104.48</v>
+      </c>
+      <c r="F51" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G51" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>4900001086.0, 4900001087.0</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>20221123</t>
+        </is>
+      </c>
+      <c r="K51" t="n">
+        <v>104.48</v>
+      </c>
+      <c r="L51" t="n">
+        <v>20896</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>SSDPF2NV017TZES</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS R VE PRQ2</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>ADPR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>26.87</v>
+      </c>
+      <c r="F52" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G52" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>4900000338.0</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>20220808.0</t>
+        </is>
+      </c>
+      <c r="K52" t="n">
+        <v>26.87</v>
+      </c>
+      <c r="L52" t="n">
+        <v>1182.28</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>SSDPF2NV153TZN1</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS R VE</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>ADPR VE</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>100.89</v>
+      </c>
+      <c r="F53" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G53" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>4900001449</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>20230313</t>
+        </is>
+      </c>
+      <c r="K53" t="n">
+        <v>100.89</v>
+      </c>
+      <c r="L53" t="n">
+        <v>22599.36</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>SSDPF2NV307TZN1</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS R VE</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>ADPR VE</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>101.36</v>
+      </c>
+      <c r="F54" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G54" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>4900001451</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>20230313</t>
+        </is>
+      </c>
+      <c r="K54" t="n">
+        <v>101.36</v>
+      </c>
+      <c r="L54" t="n">
+        <v>23110.08</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>SSDPFCKE064T1S1</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS RR ME</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>ADPRR ME PRQ1</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>69.96499999999999</v>
+      </c>
+      <c r="F55" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G55" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>4900001066.0, 4900001067.0</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>20221123.0</t>
+        </is>
+      </c>
+      <c r="K55" t="n">
+        <v>69.96499999999999</v>
+      </c>
+      <c r="L55" t="n">
+        <v>13993</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>SSDPFKNU512GZ1S</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>ECHO HARBOR PRQ1</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>EH</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="F56" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G56" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>4900001188.0</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>20230106.0</t>
+        </is>
+      </c>
+      <c r="K56" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="L56" t="n">
+        <v>1060.8</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>SSDPFUKX019T1AP</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS RR SE</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>ADPRR SE</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>53.06999999999999</v>
+      </c>
+      <c r="F57" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G57" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>4900001083.0</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>20221123</t>
+        </is>
+      </c>
+      <c r="K57" t="n">
+        <v>53.06999999999999</v>
+      </c>
+      <c r="L57" t="n">
+        <v>424.5599999999999</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>SSDPFUKX076T1AP</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS RR SE</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>ADPRR SE</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>58.67</v>
+      </c>
+      <c r="F58" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G58" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>4900001084.0</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>20221123</t>
+        </is>
+      </c>
+      <c r="K58" t="n">
+        <v>58.67</v>
+      </c>
+      <c r="L58" t="n">
+        <v>469.36</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>SSDPFWKX153T1M2</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS RR SE</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>ADPRR SE</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>108.97</v>
+      </c>
+      <c r="F59" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G59" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>4900001085.0</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>20221123</t>
+        </is>
+      </c>
+      <c r="K59" t="n">
+        <v>108.97</v>
+      </c>
+      <c r="L59" t="n">
+        <v>871.76</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>SSDPFWKX153T8M2</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>CDR SE EDSFF</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>CDR SE EDSFF</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>104.53</v>
+      </c>
+      <c r="F60" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G60" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>4900000912.0</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>20221028</t>
+        </is>
+      </c>
+      <c r="K60" t="n">
+        <v>104.53</v>
+      </c>
+      <c r="L60" t="n">
+        <v>1254.36</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>SSDPFWNV153TZES</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>NPSG PATHFINDING</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>PF</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>229.45</v>
+      </c>
+      <c r="F61" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G61" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>9000000069.0, 9000003704.0</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>20230123.0, 20230109.0</t>
+        </is>
+      </c>
+      <c r="K61" t="n">
+        <v>229.45</v>
+      </c>
+      <c r="L61" t="n">
+        <v>917.8000000000001</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>SSDPFWNV153TZM2</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS R VE</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>ADPR VE</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>101.7</v>
+      </c>
+      <c r="F62" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G62" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>4900001448</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>20230313</t>
+        </is>
+      </c>
+      <c r="K62" t="n">
+        <v>101.7</v>
+      </c>
+      <c r="L62" t="n">
+        <v>23187.6</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>SSDPFWNV307TZM2</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>ARBORDALE PLUS R VE</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>ADPR VE</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>102.17</v>
+      </c>
+      <c r="F63" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G63" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>4900001450</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>20230313</t>
+        </is>
+      </c>
+      <c r="K63" t="n">
+        <v>102.17</v>
+      </c>
+      <c r="L63" t="n">
+        <v>23703.44</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>SSDPHAKX012TZES</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>NPSG PATHFINDING</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>PF</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>181.3766666666667</v>
+      </c>
+      <c r="F64" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G64" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>4900001189.0, 9000003704.0</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>20230112.0, 20230109.0</t>
+        </is>
+      </c>
+      <c r="K64" t="n">
+        <v>105.9793333333333</v>
+      </c>
+      <c r="L64" t="n">
+        <v>2119.586666666667</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>SSDPHAKX025TZES</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>NPSG PATHFINDING</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>PF</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>112.5733333333333</v>
+      </c>
+      <c r="F65" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G65" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>4900000443.0, 4900001201.0, 4900001416.0</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>20220927.0, 20230112.0, 20230207.0</t>
+        </is>
+      </c>
+      <c r="K65" t="n">
+        <v>104.76</v>
+      </c>
+      <c r="L65" t="n">
+        <v>1815.84</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>SSDSC2KB038TZ01</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>YOUNGSVILLE RR SE</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>YV RR SE</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>21.69</v>
+      </c>
+      <c r="F66" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G66" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>4900000534, 4900000535</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>20220908</t>
+        </is>
+      </c>
+      <c r="K66" t="n">
+        <v>21.68999999999999</v>
+      </c>
+      <c r="L66" t="n">
+        <v>2342.52</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>SSDSC2KB076TZ01</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>YOUNGSVILLE RR SE</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>YV RR SE</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>22.09</v>
+      </c>
+      <c r="F67" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G67" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>4900001040, 4900001041, 4900001038, 4900001039</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>20220915, 20220908</t>
+        </is>
+      </c>
+      <c r="K67" t="n">
+        <v>22.09</v>
+      </c>
+      <c r="L67" t="n">
+        <v>2054.37</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
           <t>SSDSC2KB960GZ01</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B68" t="inlineStr">
         <is>
           <t>YOUNGSVILLE RR SE</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
         <is>
           <t>YV RR SE</t>
         </is>
       </c>
-      <c r="E45" t="n">
+      <c r="E68" t="n">
         <v>21.64</v>
       </c>
-      <c r="F45" t="n">
-        <v>202241</v>
-      </c>
-      <c r="G45" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr">
+      <c r="F68" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G68" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
         <is>
           <t>4900000536, 4900000537</t>
         </is>
       </c>
-      <c r="J45" t="inlineStr">
+      <c r="J68" t="inlineStr">
         <is>
           <t>20220908</t>
         </is>
       </c>
-      <c r="K45" t="n">
+      <c r="K68" t="n">
         <v>21.64</v>
       </c>
-      <c r="L45" t="n">
+      <c r="L68" t="n">
         <v>2337.12</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>NPSG PATHFINDING</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>PF</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>196.6</v>
+      </c>
+      <c r="F69" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G69" t="n">
+        <v>202313</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>4900001408.0, 4900001488.0</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>20230303.0, 20230317.0</t>
+        </is>
+      </c>
+      <c r="K69" t="n">
+        <v>84.41714285714286</v>
+      </c>
+      <c r="L69" t="n">
+        <v>2363.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>